<commit_message>
Added data driven for array and stack
</commit_message>
<xml_diff>
--- a/src/test/resources/Excelsheet/Excel_sheet_for_DataDrivenTesting.xlsx
+++ b/src/test/resources/Excelsheet/Excel_sheet_for_DataDrivenTesting.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\eclipse-workspace\Numpy_Dsalgo\src\test\resources\Excelsheet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0296C9E9-CD04-4287-B563-2F263D16460B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Login1" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Register" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="phythoncode" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="practice Questions" sheetId="5" r:id="rId8"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Login1" sheetId="2" r:id="rId2"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
+    <sheet name="phythoncode" sheetId="4" r:id="rId4"/>
+    <sheet name="practice Questions" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
   <si>
     <t>Username</t>
   </si>
@@ -70,9 +80,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>navtej@12</t>
     </r>
@@ -202,60 +213,202 @@
   </si>
   <si>
     <t>No tests were collected</t>
+  </si>
+  <si>
+    <t>PythonCode</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>print("hello");</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+if(num in input_list):
+print("Element Found")
+\b
+\b
+else:
+print("Not Found")
+\b
+\b
+\b
+\b
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+if(num in input_list):
+output = ("Element Found")
+\b
+\b
+else:
+output = ("Not Found")
+\b
+\b
+return(output)</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+count = 0
+result = 0
+for i in range(0, len(nums)):
+if (nums[i] == 0):
+count = 0
+\b
+\b
+else:
+count+= 1
+\b
+\b
+result = max(result, count)
+\b
+\b
+print(result)
+\b
+\b
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+max_count = 0
+current_count = 0
+for num in nums:
+if num == 1:
+current_count += 1
+max_count = max(max_count, current_count)
+\b
+\b
+else:
+current_count = 0
+#\b\b\b
+\b
+\b
+\b
+\b
+return max_count</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+c=0
+for i in nums:
+j=str(i)
+x=len(j)
+if x%2==0:
+c=c+1
+\b
+\b
+\b
+\b
+print c
+return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):return sum(len(str(num)) % 2 == 0 for num in nums)</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+\b
+\b
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list;
+return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Consolas"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial, sans-serif"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -263,7 +416,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -279,103 +432,79 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="24">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{E34F87AA-497C-4EAA-BD29-5E5892F7904E}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{84D0421A-42FD-4A9C-9543-B1D77C13CC4B}"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -565,23 +694,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="29.75"/>
+    <col min="3" max="3" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,7 +725,7 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -604,39 +736,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4">
       <c r="C6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4">
       <c r="C7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4">
       <c r="C8" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="25.25"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -658,7 +791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -669,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -680,7 +813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -688,7 +821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -696,33 +829,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3">
       <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.25"/>
-    <col customWidth="1" min="2" max="2" width="27.25"/>
-    <col customWidth="1" min="3" max="3" width="23.38"/>
-    <col customWidth="1" min="4" max="4" width="36.13"/>
+    <col min="1" max="1" width="26.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -736,233 +870,235 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="9" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="13">
-        <v>123185.0</v>
-      </c>
-      <c r="C7" s="13">
-        <v>123185.0</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="B7" s="10">
+        <v>123185</v>
+      </c>
+      <c r="C7" s="10">
+        <v>123185</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+    <row r="13" spans="1:4">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:C5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B3"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.38"/>
-    <col customWidth="1" min="2" max="2" width="37.75"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -970,7 +1106,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -978,7 +1114,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -986,138 +1122,248 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="134.63"/>
-    <col customWidth="1" min="2" max="2" width="30.38"/>
+    <col min="1" max="1" width="134.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:2" ht="13.2">
+      <c r="A1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:2" ht="14.4">
+      <c r="A2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="16" t="s">
+    <row r="4" spans="1:2" ht="13.2">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="18">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="18">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="20" t="s">
+      <c r="B6" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A7" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="18">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="20" t="s">
+      <c r="B7" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A8" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="18">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="20" t="s">
+      <c r="B8" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A9" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A11" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="16" t="s">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A12" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="20" t="s">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A13" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A14" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="15" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA62227-FDAE-4F71-AD4E-C8065C5E618A}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="60.77734375" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.8">
+      <c r="A1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.8">
+      <c r="A2" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.8">
+      <c r="A3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.4">
+      <c r="A4" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.4">
+      <c r="A5" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.4">
+      <c r="A6" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.4">
+      <c r="A7" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.4">
+      <c r="A8" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.4">
+      <c r="A9" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.4">
+      <c r="A10" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.4">
+      <c r="A11" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated register message in excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/Excelsheet/Excel_sheet_for_DataDrivenTesting.xlsx
+++ b/src/test/resources/Excelsheet/Excel_sheet_for_DataDrivenTesting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\eclipse-workspace\Numpy_Dsalgo\src\test\resources\Excelsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\araja\eclipse-workspace\Numpy_Dsalgo\src\test\resources\Excelsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0296C9E9-CD04-4287-B563-2F263D16460B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE25D10-449E-4243-833E-6CB6983FB900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
   <si>
     <t>Username</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Message</t>
-  </si>
-  <si>
-    <t>UserName cannot be blank</t>
   </si>
   <si>
     <t>`</t>
@@ -95,58 +92,31 @@
     <t>vidya</t>
   </si>
   <si>
-    <t>Passwords cannot be blank</t>
-  </si>
-  <si>
     <t>veena@12</t>
   </si>
   <si>
-    <t>password confirmation cannot be blank</t>
-  </si>
-  <si>
     <t>veena*2$</t>
   </si>
   <si>
-    <t>characters other than Letters, digits and @/./+/-/_ are not allowed</t>
-  </si>
-  <si>
-    <t>Passwords cannot be numeric</t>
-  </si>
-  <si>
     <t>divya</t>
   </si>
   <si>
     <t>priya</t>
   </si>
   <si>
-    <t>password must contain at least 8 characters</t>
-  </si>
-  <si>
     <t>kanaka@23</t>
   </si>
   <si>
     <t>kanaka@12</t>
   </si>
   <si>
-    <t>Passwords cannot be different</t>
-  </si>
-  <si>
     <t>praveena</t>
   </si>
   <si>
     <t>praveena12</t>
   </si>
   <si>
-    <t>Passwords cannot be similar to full name or any additions to name</t>
-  </si>
-  <si>
     <t>welcome@123</t>
-  </si>
-  <si>
-    <t>Common passwords cannot be used</t>
-  </si>
-  <si>
-    <t>Login successfull</t>
   </si>
   <si>
     <t>pythoncode</t>
@@ -324,12 +294,18 @@
 return sorted_squares_list;
 sortedSquares([-7,-3,2,3,11])</t>
   </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>New Account Created. You are logged in as &lt;username&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -408,6 +384,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -445,7 +427,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -477,13 +459,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,14 +829,16 @@
   </sheetPr>
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26.21875" customWidth="1"/>
     <col min="2" max="2" width="27.21875" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="53.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -874,63 +859,63 @@
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="6" t="s">
-        <v>15</v>
+      <c r="D2" s="24" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="6" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="6" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="10">
         <v>123185</v>
@@ -939,68 +924,68 @@
         <v>123185</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>4</v>
@@ -1009,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1100,18 +1085,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1119,7 +1104,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1150,26 +1135,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="13.2">
       <c r="A1" s="12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.4">
       <c r="A2" s="18" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="13" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.2">
@@ -1178,7 +1163,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B5" s="15">
         <v>2</v>
@@ -1186,7 +1171,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B6" s="15">
         <v>3</v>
@@ -1194,7 +1179,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="17" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B7" s="15">
         <v>2</v>
@@ -1202,7 +1187,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B8" s="15">
         <v>1</v>
@@ -1210,50 +1195,50 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="17" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="17" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1">
       <c r="A11" s="13" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1">
       <c r="A13" s="17" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="17" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1265,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA62227-FDAE-4F71-AD4E-C8065C5E618A}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1276,91 +1261,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.8">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.8">
+      <c r="A2" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.8">
+      <c r="A3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.4">
+      <c r="A4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.4">
+      <c r="A5" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.4">
+      <c r="A6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.4">
+      <c r="A7" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.4">
+      <c r="A8" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.4">
+      <c r="A9" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.4">
+      <c r="A10" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="13.8">
-      <c r="A3" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.4">
-      <c r="A4" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.4">
-      <c r="A5" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.4">
-      <c r="A6" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.4">
-      <c r="A7" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.4">
-      <c r="A8" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.4">
-      <c r="A9" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="14.4">
-      <c r="A10" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>54</v>
+      <c r="B10" s="21" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.4">
-      <c r="A11" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>58</v>
+      <c r="A11" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated POM,clean up code
</commit_message>
<xml_diff>
--- a/src/test/resources/Excelsheet/Excel_sheet_for_DataDrivenTesting.xlsx
+++ b/src/test/resources/Excelsheet/Excel_sheet_for_DataDrivenTesting.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\araja\eclipse-workspace\Numpy_Dsalgo\src\test\resources\Excelsheet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027A131F-5653-4B3D-8B28-1224C962DED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Login1" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Register" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="phythoncode" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="practice Questions" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Sheet1" sheetId="6" r:id="rId9"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Login1" sheetId="2" r:id="rId2"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
+    <sheet name="phythoncode" sheetId="4" r:id="rId4"/>
+    <sheet name="practice Questions" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="4ZaeplFR2A/tUPZFB1QgVyeRAZ6oTbhUuVPEwxXSvR0="/>
@@ -21,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
   <si>
     <t>Username</t>
   </si>
@@ -70,10 +79,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="10.0"/>
-        <u/>
       </rPr>
       <t>navtej@12</t>
     </r>
@@ -89,9 +98,6 @@
   </si>
   <si>
     <t>veena*2$</t>
-  </si>
-  <si>
-    <t>password_mismatch:The two password fields didn’t match.</t>
   </si>
   <si>
     <t>divya</t>
@@ -293,42 +299,75 @@
 return sorted_squares_list;
 sortedSquares([-7,-3,2,3,11])</t>
   </si>
+  <si>
+    <t>characters other than Letters, digits and @/./+/-/_ are not allowed</t>
+  </si>
+  <si>
+    <t>Passwords cannot be numeric</t>
+  </si>
+  <si>
+    <t>password must contain at least 8 characters</t>
+  </si>
+  <si>
+    <t>Passwords cannot be different</t>
+  </si>
+  <si>
+    <t>Passwords cannot be similar to full name or any additions to name</t>
+  </si>
+  <si>
+    <t>Common passwords cannot be used</t>
+  </si>
+  <si>
+    <t>Please enter valid data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Consolas"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial, sans-serif"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -336,7 +375,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -351,85 +390,98 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -619,26 +671,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="12.63"/>
-    <col customWidth="1" min="3" max="3" width="29.75"/>
-    <col customWidth="1" min="4" max="6" width="12.63"/>
+    <col min="1" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.77734375" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,7 +704,7 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -661,30 +715,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1670,30 +1724,28 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="12.63"/>
-    <col customWidth="1" min="3" max="3" width="25.25"/>
-    <col customWidth="1" min="4" max="6" width="12.63"/>
+    <col min="1" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1704,7 +1756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1715,7 +1767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1726,7 +1778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1737,7 +1789,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1745,7 +1797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1753,20 +1805,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -2752,32 +2804,30 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.25"/>
-    <col customWidth="1" min="2" max="2" width="27.25"/>
-    <col customWidth="1" min="3" max="3" width="23.38"/>
-    <col customWidth="1" min="4" max="4" width="53.25"/>
-    <col customWidth="1" min="5" max="6" width="12.63"/>
+    <col min="1" max="1" width="26.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="55.88671875" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -2791,7 +2841,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2799,7 +2849,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="3" t="s">
         <v>15</v>
@@ -2811,7 +2861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -2821,18 +2871,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="18" t="s">
         <v>18</v>
       </c>
+      <c r="C5" s="19"/>
       <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -2842,81 +2893,81 @@
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
+      <c r="D6" s="16" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="6">
-        <v>123185.0</v>
+        <v>123185</v>
       </c>
       <c r="C7" s="6">
-        <v>123185.0</v>
-      </c>
-      <c r="D7" s="3" t="s">
+        <v>123185</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3" t="s">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -2927,77 +2978,77 @@
         <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -3970,69 +4021,71 @@
   <mergeCells count="1">
     <mergeCell ref="B5:C5"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.38"/>
-    <col customWidth="1" min="2" max="2" width="37.75"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.77734375" customWidth="1"/>
+    <col min="3" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="3"/>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B4" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -5018,139 +5071,137 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="134.63"/>
-    <col customWidth="1" min="2" max="2" width="30.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
+    <col min="1" max="1" width="134.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>35</v>
       </c>
+      <c r="B2" s="10" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="10" t="s">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A3" s="11" t="s">
         <v>37</v>
       </c>
+      <c r="B3" s="12" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="12">
-        <v>2.0</v>
+      <c r="B6" s="12">
+        <v>3</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="12">
-        <v>3.0</v>
+      <c r="B7" s="12">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="13" t="s">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A8" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="12">
-        <v>2.0</v>
+      <c r="B8" s="12">
+        <v>1</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="13" t="s">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="12">
-        <v>1.0</v>
+      <c r="B9" s="12" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="12" t="s">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A10" s="13" t="s">
         <v>45</v>
       </c>
+      <c r="B10" s="12" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="12" t="s">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="12" t="s">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>48</v>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -6136,121 +6187,117 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="60.75"/>
-    <col customWidth="1" min="2" max="2" width="45.88"/>
-    <col customWidth="1" min="3" max="26" width="8.63"/>
+    <col min="1" max="1" width="60.77734375" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" customWidth="1"/>
+    <col min="3" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1">
+    <row r="1" spans="1:2" ht="12.75" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
+    <row r="3" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
+      <c r="B4" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>32</v>
+    <row r="5" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>37</v>
+    <row r="6" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A6" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>49</v>
+    <row r="7" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A7" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="14" t="s">
+    <row r="8" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>49</v>
+    <row r="9" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A9" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>57</v>
+    <row r="10" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A10" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="14" t="s">
+    <row r="11" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>49</v>
+      <c r="B11" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" ht="12.75" customHeight="1"/>
-    <row r="13" ht="12.75" customHeight="1"/>
-    <row r="14" ht="12.75" customHeight="1"/>
-    <row r="15" ht="12.75" customHeight="1"/>
-    <row r="16" ht="12.75" customHeight="1"/>
+    <row r="12" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="13" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="14" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="15" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="16" spans="1:2" ht="12.75" customHeight="1"/>
     <row r="17" ht="12.75" customHeight="1"/>
     <row r="18" ht="12.75" customHeight="1"/>
     <row r="19" ht="12.75" customHeight="1"/>
@@ -7236,9 +7283,7 @@
     <row r="999" ht="12.75" customHeight="1"/>
     <row r="1000" ht="12.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>